<commit_message>
Updated test data for TC 51999,51987,51990
</commit_message>
<xml_diff>
--- a/Test Data/TC_51987_Verify_If_Panel_Type_Dropdown_Is_Filtered_Based_On_The_Slotcard_Positions_Occupied.xlsx
+++ b/Test Data/TC_51987_Verify_If_Panel_Type_Dropdown_Is_Filtered_Based_On_The_Slotcard_Positions_Occupied.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\work\consys-uiauto\Test Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{099D83EF-7492-4787-9134-D7B7E12057BD}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5563A18-7E99-4F24-826E-B001F1F447BC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="46">
   <si>
     <t>Color Codes</t>
   </si>
@@ -600,8 +600,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F7" workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -852,11 +852,11 @@
       <c r="K10" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L10" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M10" s="14" t="s">
-        <v>23</v>
+      <c r="L10" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M10" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="N10" s="14" t="s">
         <v>35</v>
@@ -908,11 +908,11 @@
       <c r="K11" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="M11" s="14" t="s">
-        <v>23</v>
+      <c r="L11" s="14" t="b">
+        <v>0</v>
+      </c>
+      <c r="M11" s="14" t="b">
+        <v>0</v>
       </c>
       <c r="N11" s="14" t="s">
         <v>35</v>

</xml_diff>